<commit_message>
kick PARTNER from project group for AUTHORs and ADMINs
</commit_message>
<xml_diff>
--- a/usersList.xlsx
+++ b/usersList.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,20 +487,30 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>speciality</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>group</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>phonenum</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>email</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>projectMember</t>
         </is>
@@ -534,7 +544,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>ахахахахах</t>
+          <t>Программист</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -559,34 +569,39 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>Инжиниринг предприятий и информационных систем</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>ПИ03у</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
           <t>+79993332211</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>ivanov.i.i@gmail.com</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>{EVENT_MANAGER,RESIDENT,ADMIN}</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>dfg</t>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>{RESIDENT,ADMIN,EVENT_MANAGER}</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>TimeTrace</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>riba17</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Кабанов</t>
+          <t>whereistheexit</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -594,17 +609,17 @@
           <t>Илья</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>{RESIDENT}</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>whereistheexit</t>
+          <t>riba17</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -612,12 +627,12 @@
           <t>Илья</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>{RESIDENT}</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>